<commit_message>
Nueva característica, +datos, matrices de correlación
</commit_message>
<xml_diff>
--- a/reports/tags-2.xlsx
+++ b/reports/tags-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana12\Desktop\TFG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana12\Desktop\TFG\git\TFG\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1E2AA2-5A4E-44D1-B388-B6FA5AAD1B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5B487B-F5C2-4253-8ED2-8623510D5C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14970" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -294,7 +294,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,8 +335,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,11 +643,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="151" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
@@ -1421,162 +1427,162 @@
         <v>2.2657004830918002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>205</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>172</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>174.10624911863999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>51.830877847457998</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>283</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>177</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>47.367231638417998</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>3</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <v>4.6497175141243003</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="2">
         <v>20</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="2">
         <v>2</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
         <v>5.6666666666666998</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="2">
         <v>36</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="2">
         <v>1</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <v>14.468926553672</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="2">
         <v>142</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="2">
         <v>1</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="2">
         <v>4.0225988700565001</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="2">
         <v>61</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="2">
         <v>1.3446327683616</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="2">
         <v>13.717514124294</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="2">
         <v>0.28248587570620998</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="2">
         <v>2.6553672316384</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>185</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>174</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>119.27156864972</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>13.211298666667</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>207</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>177</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>32.830508474576</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="2">
         <v>3</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="2">
         <v>3.8813559322033999</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="2">
         <v>18</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
         <v>0.54237288135592998</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="2">
         <v>20</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="2">
         <v>1</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="2">
         <v>9.8531073446328001</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="2">
         <v>70</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="2">
         <v>3</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="2">
         <v>8.7683615819208995</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="2">
         <v>59</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="2">
         <v>0.39548022598869997</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="2">
         <v>6.8757062146893002</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="2">
         <v>0.2090395480226</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="2">
         <v>1.5875706214689</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
       <c r="B13">
@@ -1652,157 +1658,157 @@
         <v>2.8292682926829</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>179</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>151</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>151.88849066447</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>33.851191098683998</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>234</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>152</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>45.256578947367998</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="2">
         <v>5</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="2">
         <v>5.6381578947367998</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="2">
         <v>24</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="2">
         <v>8</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="2">
         <v>18.25</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="2">
         <v>153</v>
       </c>
-      <c r="P14">
-        <v>2</v>
-      </c>
-      <c r="Q14">
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
         <v>7.9539473684211002</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="2">
         <v>83</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
         <v>1.1118421052631999</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="2">
         <v>67</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="2">
         <v>0.23684210526315999</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="2">
         <v>8.7171052631578991</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="2">
         <v>0.42105263157895001</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="2">
         <v>1.7302631578947001</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>175</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>141</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>183.33560147944999</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>26.335035780822</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>249</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>146</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>53.493150684931997</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>4</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <v>4.5410958904110004</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>16</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="2">
         <v>4</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="2">
         <v>20.150684931507001</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="2">
         <v>213</v>
       </c>
-      <c r="P15" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3">
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
         <v>7.0753424657534003</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="2">
         <v>104</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15" s="2">
         <v>1</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15" s="2">
         <v>7.6849315068493</v>
       </c>
-      <c r="U15" s="3">
+      <c r="U15" s="2">
         <v>90</v>
       </c>
-      <c r="V15" s="3">
+      <c r="V15" s="2">
         <v>0.26712328767123</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15" s="2">
         <v>7.9383561643835998</v>
       </c>
-      <c r="X15" s="3">
+      <c r="X15" s="2">
         <v>1.6095890410959</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y15" s="2">
         <v>3.0205479452055002</v>
       </c>
     </row>
@@ -2037,80 +2043,80 @@
         <v>4.4864864864865002</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>148</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>110</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>116.10769860000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>48.512790572726999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>201</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>110</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>31.109090909091002</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>3</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="3">
         <v>4.6636363636364004</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <v>25</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="3">
         <v>4</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="3">
         <v>7.0636363636363999</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <v>47</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="3">
         <v>1</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <v>6.0545454545455</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="3">
         <v>73</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="3">
         <v>1</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="3">
         <v>2.7272727272727</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="3">
         <v>22</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="3">
         <v>0.84545454545455001</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="3">
         <v>6.6090909090908996</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="3">
         <v>0.85454545454544995</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="3">
         <v>1.8</v>
       </c>
     </row>
@@ -2269,7 +2275,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>83</v>
       </c>
       <c r="B22">

</xml_diff>